<commit_message>
so far so good
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Settlements.xlsx
+++ b/OpenWorld/Resources/Settlements.xlsx
@@ -98,12 +98,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -127,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -436,23 +446,24 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -678,5 +689,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>